<commit_message>
addvertiesments & profile pic done
update profile pic thing has done
</commit_message>
<xml_diff>
--- a/requiredFiles/ResultSheet.xlsx
+++ b/requiredFiles/ResultSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Editing\requiredFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Editing\requiredFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,12 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>IndexNo</t>
-  </si>
-  <si>
-    <t>Name</t>
   </si>
   <si>
     <t>Marks</t>
@@ -38,15 +35,12 @@
   <si>
     <t>17XXXS</t>
   </si>
-  <si>
-    <t>Sample Name</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,18 +57,12 @@
     </font>
     <font>
       <sz val="14"/>
-      <color theme="1"/>
-      <name val="Bookman Old Style"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="14"/>
       <color theme="0"/>
       <name val="Bookman Old Style"/>
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -84,12 +72,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -107,18 +89,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -405,48 +384,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="45.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B2" s="4">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="5">
-        <v>25</v>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="4">
+        <v>35.5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C3" s="5">
-        <v>35.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C4" s="5">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="4">
         <v>25.6</v>
       </c>
     </row>

</xml_diff>